<commit_message>
Updated scaling of all maps, including props inside Level 1. Deleted many back faces on architecture geo in level 1.
</commit_message>
<xml_diff>
--- a/Work In Progress/ModelsGanttChart.xlsx
+++ b/Work In Progress/ModelsGanttChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackgoodman\Desktop\SeniorProject\SeniorProject\Work In Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BBEB49A-6A8F-46FD-B38E-2BDBA4EEA0E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DADF916-0935-4291-A164-639EB917FF28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{EE7AD68D-AD29-4A9C-A3A6-1670892AA766}"/>
   </bookViews>
@@ -181,7 +181,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,6 +230,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -243,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -259,6 +265,8 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4004672F-2106-433B-A4AA-04FA5F8E4B17}">
-  <dimension ref="A1:AQ69"/>
+  <dimension ref="A1:AQ59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AM11" sqref="AM11"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,6 +696,13 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
       <c r="AP3" s="12" t="s">
         <v>39</v>
       </c>
@@ -697,6 +712,13 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
       <c r="AP4" s="11"/>
       <c r="AQ4" s="11"/>
     </row>
@@ -704,6 +726,13 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
       <c r="AP5" s="11"/>
       <c r="AQ5" s="11"/>
     </row>
@@ -711,6 +740,13 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
       <c r="AP6" s="11"/>
       <c r="AQ6" s="11"/>
     </row>
@@ -718,6 +754,13 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
       <c r="AP7" s="11"/>
       <c r="AQ7" s="11"/>
     </row>
@@ -741,6 +784,20 @@
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
       <c r="AP12" s="11"/>
       <c r="AQ12" s="11"/>
     </row>
@@ -818,6 +875,27 @@
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
       <c r="AP26" s="11"/>
       <c r="AQ26" s="11"/>
     </row>
@@ -903,6 +981,34 @@
       <c r="A42" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+      <c r="T42" s="3"/>
+      <c r="U42" s="3"/>
+      <c r="V42" s="3"/>
+      <c r="W42" s="3"/>
+      <c r="X42" s="3"/>
+      <c r="Y42" s="3"/>
+      <c r="Z42" s="3"/>
+      <c r="AA42" s="3"/>
+      <c r="AB42" s="3"/>
+      <c r="AC42" s="3"/>
       <c r="AP42" s="11"/>
       <c r="AQ42" s="11"/>
     </row>
@@ -948,40 +1054,105 @@
       <c r="AP48" s="11"/>
       <c r="AQ48" s="11"/>
     </row>
-    <row r="51" spans="1:1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AP49" s="14"/>
+      <c r="AQ49" s="14"/>
+    </row>
+    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AP50" s="14"/>
+      <c r="AQ50" s="14"/>
+    </row>
+    <row r="51" spans="1:43" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="3"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="3"/>
+      <c r="T51" s="3"/>
+      <c r="U51" s="3"/>
+      <c r="V51" s="3"/>
+      <c r="W51" s="3"/>
+      <c r="X51" s="3"/>
+      <c r="Y51" s="3"/>
+      <c r="Z51" s="3"/>
+      <c r="AA51" s="3"/>
+      <c r="AB51" s="3"/>
+      <c r="AC51" s="3"/>
+      <c r="AD51" s="3"/>
+      <c r="AE51" s="3"/>
+      <c r="AF51" s="3"/>
+      <c r="AG51" s="3"/>
+      <c r="AH51" s="3"/>
+      <c r="AI51" s="3"/>
+      <c r="AJ51" s="3"/>
+      <c r="AP51" s="14"/>
+      <c r="AQ51" s="14"/>
+    </row>
+    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="AP52" s="14"/>
+      <c r="AQ52" s="14"/>
+    </row>
+    <row r="53" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AP53" s="14"/>
+      <c r="AQ53" s="14"/>
+    </row>
+    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AP54" s="14"/>
+      <c r="AQ54" s="14"/>
+    </row>
+    <row r="55" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="10" t="s">
+      <c r="AP55" s="14"/>
+      <c r="AQ55" s="14"/>
+    </row>
+    <row r="56" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="9" t="s">
+      <c r="AP56" s="14"/>
+      <c r="AQ56" s="14"/>
+    </row>
+    <row r="57" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="8" t="s">
+      <c r="AP57" s="14"/>
+      <c r="AQ57" s="14"/>
+    </row>
+    <row r="58" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
+      <c r="AP58" s="14"/>
+      <c r="AQ58" s="14"/>
+    </row>
+    <row r="59" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
         <v>34</v>
       </c>
+      <c r="AP59" s="14"/>
+      <c r="AQ59" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>